<commit_message>
colunas criadas no quadro e scroll a funcionar
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B0DFC2-572F-6646-9D57-6B4F8DA01860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE34DBF2-6633-E74E-9873-503DC35FB615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>Catergoria</t>
   </si>
@@ -297,6 +297,9 @@
       </rPr>
       <t>login</t>
     </r>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -875,7 +878,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -918,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
troca de vídeo de fundo por imagem
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D840EF-A47F-AA4C-9ADB-A7DA32F5C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F912AFC-1B28-6341-8C2B-EB3E6AD24EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,12 +361,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
@@ -401,6 +395,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -605,29 +605,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -641,29 +632,38 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +887,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -906,285 +906,285 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>8</v>
+      <c r="E9" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>8</v>
+      <c r="E15" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Merge branch 'nomeLoginEntrar'"
This reverts commit 35987144ec4d4749bc17e13bf7e93acd6df0edeb, reversing
changes made to 70f2c520f77508001df898876c6806f8c505475b.
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F912AFC-1B28-6341-8C2B-EB3E6AD24EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D840EF-A47F-AA4C-9ADB-A7DA32F5C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,6 +361,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
@@ -395,12 +401,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -605,20 +605,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -632,38 +641,29 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +887,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -906,285 +906,285 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>29</v>
+      <c r="E9" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>29</v>
+      <c r="E15" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="21" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'nomeLoginEntrar'""
This reverts commit 8d6cda7ae5db00e2a61a9043a1e1b2a9f250c7f6.
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D840EF-A47F-AA4C-9ADB-A7DA32F5C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F912AFC-1B28-6341-8C2B-EB3E6AD24EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,12 +361,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
@@ -401,6 +395,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -605,29 +605,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -641,29 +632,38 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +887,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -906,285 +906,285 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>8</v>
+      <c r="E9" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>8</v>
+      <c r="E15" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Merge branch 'nomeLoginEntrar'"""
This reverts commit 81356bae74921071504ee2a5c4493b97ba0b35ef.
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F912AFC-1B28-6341-8C2B-EB3E6AD24EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D840EF-A47F-AA4C-9ADB-A7DA32F5C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,6 +361,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
@@ -395,12 +401,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -605,20 +605,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -632,38 +641,29 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +887,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -906,285 +906,285 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>29</v>
+      <c r="E9" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>29</v>
+      <c r="E15" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="21" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
alertas de teste retirados
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D840EF-A47F-AA4C-9ADB-A7DA32F5C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65545B98-2ACB-8348-A146-E06D97297452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -339,8 +339,15 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,12 +364,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE6B8AF"/>
         <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -401,6 +402,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF277E40"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -597,73 +610,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +903,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -900,291 +916,291 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>8</v>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>8</v>
+      <c r="D10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>8</v>
+      <c r="D11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>8</v>
+      <c r="E14" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>8</v>
+      <c r="E15" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2176,7 +2192,7 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E13 E16:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Não iniciado,Em execução,Terminado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
JS para o login
</commit_message>
<xml_diff>
--- a/Ficheiros/Requisitos projecto 1.xlsx
+++ b/Ficheiros/Requisitos projecto 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardoelias/Desktop/Projeto1/Projeto1_Scrum/Ficheiros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65545B98-2ACB-8348-A146-E06D97297452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0429FDC3-D81B-4448-A7CB-A7E2BB295E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,12 +610,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -645,12 +642,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -675,11 +666,17 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,7 +900,7 @@
   <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -916,101 +913,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1018,16 +1015,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1035,101 +1032,101 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1137,71 +1134,71 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>8</v>
+      <c r="E17" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2192,7 +2189,7 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E13 E16:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Não iniciado,Em execução,Terminado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>